<commit_message>
HD BOM info added
</commit_message>
<xml_diff>
--- a/bom/BOM_XYHD12.xlsx
+++ b/bom/BOM_XYHD12.xlsx
@@ -5,22 +5,32 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{1482C30D-B79B-4A5C-88E7-33DF6EF428FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{80E5BCD1-3E2F-4946-BC04-9E06745423EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F52D8-30DC-468E-9866-7EE19291B0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="151">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -337,6 +347,130 @@
   </si>
   <si>
     <t>Motor, Servo - Nema 23</t>
+  </si>
+  <si>
+    <t>https://www.teknic.com/model-info/CPM-SDSK-2321S-RQN/?model_voltage=75</t>
+  </si>
+  <si>
+    <t>ClearPath by Teknic</t>
+  </si>
+  <si>
+    <t>Thingiverse</t>
+  </si>
+  <si>
+    <t>12mm 2GT Belt</t>
+  </si>
+  <si>
+    <t>12mm 2GT belt</t>
+  </si>
+  <si>
+    <t>BeltLower_YLH_Section</t>
+  </si>
+  <si>
+    <t>BeltUpper_YLH_Section</t>
+  </si>
+  <si>
+    <t>HD_YCarriage_RH_LowerBody</t>
+  </si>
+  <si>
+    <t>HD_YCarriage_RH_UpperBody</t>
+  </si>
+  <si>
+    <t>HD_YCarriage_LH_LowerBody</t>
+  </si>
+  <si>
+    <t>HD_YCarriage_LH_UpperBody</t>
+  </si>
+  <si>
+    <t>M3X3030_TSlot_Nut</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32917702848.html?spm=a2g0s.9042311.0.0.10194c4dtWXsMc</t>
+  </si>
+  <si>
+    <t>M3X2020_T-Nut</t>
+  </si>
+  <si>
+    <t>Nut, TSlot - M3X2020 For X Axis</t>
+  </si>
+  <si>
+    <t>Qty 8 based on X&amp;Y Print size at 315.  Add Qty1 for every additional 5cm of Y axis over 315mm.  (one every two holes)</t>
+  </si>
+  <si>
+    <t>Nut, TSlot - M3X3030 for Y Axis</t>
+  </si>
+  <si>
+    <t>Qty 24 based on X&amp;Y Print size at 315.  Add Qty2 (one per Y side) for every additional 5cm of Y axis over 315mm.  (one every 2 holes)</t>
+  </si>
+  <si>
+    <t>Track_HD_X_2020Profile</t>
+  </si>
+  <si>
+    <t>M3X10_CapScrew_92290A115</t>
+  </si>
+  <si>
+    <t>Screw, Cap - M3X10mm</t>
+  </si>
+  <si>
+    <t>M3X8_CapScrew_92290A113</t>
+  </si>
+  <si>
+    <t>Screw, Cap - M3X8mm</t>
+  </si>
+  <si>
+    <t>https://www.thingiverse.com/thing:4625509</t>
+  </si>
+  <si>
+    <t>MGN12H Block for X and Y axis</t>
+  </si>
+  <si>
+    <t>*Length defined by Frame Calculator: https://miragec79.github.io/HevORT/framecalculator.html
+Look for HD X Cross Member into calculator</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>M5X2020_T-Nut_91239A224</t>
+  </si>
+  <si>
+    <t>Nut, T-Slot - M5 for 2020 profile</t>
+  </si>
+  <si>
+    <t>1: Amazon (Link to Canada)
+2: AliExpress</t>
+  </si>
+  <si>
+    <t>1: https://www.amazon.ca/gp/product/B01MTKNWZB/ref=ppx_yo_dt_b_asin_image_o03_s00?ie=UTF8&amp;psc=1
+2: https://www.aliexpress.com/item/4000473863693.html?spm=a2g0s.9042311.0.0.46214c4dj2VePT</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32952396111.html?spm=a2g0s.9042311.0.0.27424c4dlCkvdt</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32856629143.html?spm=a2g0s.9042311.0.0.27424c4djK3sna</t>
+  </si>
+  <si>
+    <t>GATES-LL-2GT gear synchronous belt, 12mm wide</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33023133633.html?spm=a2g0s.9042311.0.0.27424c4doxVFvb</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33023279793.html?spm=a2g0s.9042311.0.0.27424c4doxVFvb</t>
+  </si>
+  <si>
+    <t>RDC Official Store - AliExpress</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32856649040.html?spm=2114.12010612.8148356.71.2e8e17b83q00jq</t>
+  </si>
+  <si>
+    <t>1: https://www.amazon.ca/gp/product/B01MTKNWZB/ref=ppx_yo_dt_b_asin_image_o03_s00?ie=UTF8&amp;psc=1 
+2: https://www.aliexpress.com/item/4000473863693.html?spm=a2g0s.9042311.0.0.46214c4dj2VePT</t>
   </si>
   <si>
     <r>
@@ -362,99 +496,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> NEMA23 Stepper Motors are slow. You might consider to use Nema 17 High Torque from E3D using adapter plate if you are not ready for Servo Motors. </t>
+      <t xml:space="preserve"> NEMA23 Stepper Motors are slow. You might consider to use Nema 17 High Torque from E3D using adapter plate if you are not ready for Servo Motors. 
+NEMA17 Adapter Plate: https://www.thingiverse.com/thing:4629296</t>
     </r>
   </si>
   <si>
-    <t>https://www.teknic.com/model-info/CPM-SDSK-2321S-RQN/?model_voltage=75</t>
-  </si>
-  <si>
-    <t>ClearPath by Teknic</t>
-  </si>
-  <si>
-    <t>Thingiverse</t>
-  </si>
-  <si>
-    <t>12mm 2GT Belt</t>
-  </si>
-  <si>
-    <t>12mm 2GT belt</t>
-  </si>
-  <si>
-    <t>BeltLower_YLH_Section</t>
-  </si>
-  <si>
-    <t>BeltUpper_YLH_Section</t>
-  </si>
-  <si>
-    <t>HD_YCarriage_RH_LowerBody</t>
-  </si>
-  <si>
-    <t>HD_YCarriage_RH_UpperBody</t>
-  </si>
-  <si>
-    <t>HD_YCarriage_LH_LowerBody</t>
-  </si>
-  <si>
-    <t>HD_YCarriage_LH_UpperBody</t>
-  </si>
-  <si>
-    <t>M3X3030_TSlot_Nut</t>
-  </si>
-  <si>
-    <t>AliExpress</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32917702848.html?spm=a2g0s.9042311.0.0.10194c4dtWXsMc</t>
-  </si>
-  <si>
-    <t>M3X2020_T-Nut</t>
-  </si>
-  <si>
-    <t>Nut, TSlot - M3X2020 For X Axis</t>
-  </si>
-  <si>
-    <t>Qty 8 based on X&amp;Y Print size at 315.  Add Qty1 for every additional 5cm of Y axis over 315mm.  (one every two holes)</t>
-  </si>
-  <si>
-    <t>Nut, TSlot - M3X3030 for Y Axis</t>
-  </si>
-  <si>
-    <t>Qty 24 based on X&amp;Y Print size at 315.  Add Qty2 (one per Y side) for every additional 5cm of Y axis over 315mm.  (one every 2 holes)</t>
-  </si>
-  <si>
-    <t>Track_HD_X_2020Profile</t>
-  </si>
-  <si>
-    <t>M3X10_CapScrew_92290A115</t>
-  </si>
-  <si>
-    <t>Screw, Cap - M3X10mm</t>
-  </si>
-  <si>
-    <t>M3X8_CapScrew_92290A113</t>
-  </si>
-  <si>
-    <t>Screw, Cap - M3X8mm</t>
-  </si>
-  <si>
-    <t>https://www.thingiverse.com/thing:4625509</t>
-  </si>
-  <si>
-    <t>MGN12H Block for X and Y axis</t>
-  </si>
-  <si>
-    <t>*Length defined by Frame Calculator: https://miragec79.github.io/HevORT/framecalculator.html
-Look for HD X Cross Member into calculator</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>M5X2020_T-Nut_91239A224</t>
-  </si>
-  <si>
-    <t>Nut, T-Slot - M5 for 2020 profile</t>
+    <t>Specs: https://e3d-online.dozuki.com/Document/SOMXNf6bhCInuaHa/Gates_S_Idler_12T.pdf</t>
+  </si>
+  <si>
+    <t>Specs: https://e3d-online.dozuki.com/Document/qIO5SWebKKUwlRel/Gates_T_Idler_12.pdf</t>
+  </si>
+  <si>
+    <t>Specs: https://e3d-online.dozuki.com/Document/u12AYiVxLWKRQ3Xm/Gates_Pulley_20T_12.pdf</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33008007487.html?spm=a2g0s.9042311.0.0.27424c4dyaVcbb</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/33002873710.html?spm=a2g0s.9042311.0.0.79334c4dbGMssZ</t>
   </si>
 </sst>
 </file>
@@ -690,7 +749,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -804,6 +863,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3911,7 +3973,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:K7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="84.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3924,9 +3986,9 @@
     <col min="6" max="6" width="42.1796875" style="32" customWidth="1"/>
     <col min="7" max="7" width="13" style="11" customWidth="1"/>
     <col min="8" max="8" width="9.1796875" style="11"/>
-    <col min="9" max="9" width="48.08984375" style="29" customWidth="1"/>
+    <col min="9" max="9" width="60" style="29" customWidth="1"/>
     <col min="10" max="10" width="30" style="8" customWidth="1"/>
-    <col min="11" max="11" width="30.1796875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="61" style="8" customWidth="1"/>
     <col min="12" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
@@ -3991,8 +4053,12 @@
       <c r="I2" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="33"/>
+      <c r="J2" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="3" spans="1:11" s="9" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
@@ -4020,8 +4086,12 @@
       <c r="I3" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="33"/>
+      <c r="J3" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="4" spans="1:11" s="9" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
@@ -4049,8 +4119,12 @@
       <c r="I4" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="33"/>
+      <c r="J4" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
@@ -4064,10 +4138,10 @@
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>5</v>
@@ -4075,11 +4149,15 @@
       <c r="H5" s="22">
         <v>1</v>
       </c>
-      <c r="I5" s="31"/>
+      <c r="I5" s="31" t="s">
+        <v>139</v>
+      </c>
       <c r="J5" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="38" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
@@ -4093,10 +4171,10 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>5</v>
@@ -4104,13 +4182,17 @@
       <c r="H6" s="12">
         <v>1</v>
       </c>
-      <c r="I6" s="31"/>
+      <c r="I6" s="31" t="s">
+        <v>139</v>
+      </c>
       <c r="J6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="K6" s="36"/>
+      <c r="K6" s="38" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>71</v>
       </c>
@@ -4134,13 +4216,13 @@
         <v>2</v>
       </c>
       <c r="I7" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" s="36" t="s">
         <v>105</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="K7" s="36" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4169,8 +4251,12 @@
       <c r="I8" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="34"/>
+      <c r="J8" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
@@ -4198,8 +4284,12 @@
       <c r="I9" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="34"/>
+      <c r="J9" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="K9" s="33" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
@@ -4224,11 +4314,15 @@
       <c r="H10" s="12">
         <v>4</v>
       </c>
-      <c r="I10" s="13"/>
+      <c r="I10" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="J10" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="K10" s="35"/>
+      <c r="K10" s="36" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
@@ -4253,11 +4347,15 @@
       <c r="H11" s="12">
         <v>6</v>
       </c>
-      <c r="I11" s="13"/>
+      <c r="I11" s="13" t="s">
+        <v>147</v>
+      </c>
       <c r="J11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="K11" s="35"/>
+      <c r="K11" s="36" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
@@ -4280,11 +4378,15 @@
       <c r="H12" s="12">
         <v>2</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="13" t="s">
+        <v>148</v>
+      </c>
       <c r="J12" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="K12" s="35"/>
+      <c r="K12" s="36" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
@@ -4312,8 +4414,12 @@
       <c r="I13" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="35"/>
+      <c r="J13" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="K13" s="33" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
@@ -4341,8 +4447,12 @@
       <c r="I14" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="35"/>
+      <c r="J14" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" s="36" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
@@ -4417,7 +4527,7 @@
         <v>85</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>5</v>
@@ -4457,8 +4567,12 @@
       <c r="I18" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="35"/>
+      <c r="J18" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K18" s="36" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
@@ -4513,8 +4627,12 @@
       <c r="I20" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="35"/>
+      <c r="J20" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="21" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
@@ -4528,7 +4646,7 @@
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>83</v>
@@ -4540,7 +4658,7 @@
         <v>84</v>
       </c>
       <c r="I21" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J21" s="25"/>
       <c r="K21" s="34"/>
@@ -4584,10 +4702,10 @@
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" s="30" t="s">
         <v>126</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>127</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>5</v>
@@ -4596,7 +4714,7 @@
         <v>24</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="35"/>
@@ -4640,10 +4758,10 @@
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="30" t="s">
         <v>120</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>121</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>5</v>
@@ -4652,13 +4770,13 @@
         <v>8</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K25" s="35" t="s">
         <v>118</v>
-      </c>
-      <c r="K25" s="35" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4673,10 +4791,10 @@
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>5</v>
@@ -4685,13 +4803,13 @@
         <v>24</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J26" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K26" s="35" t="s">
         <v>118</v>
-      </c>
-      <c r="K26" s="35" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4760,10 +4878,10 @@
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="30" t="s">
         <v>128</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>129</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>5</v>
@@ -4772,7 +4890,7 @@
         <v>8</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J29" s="9"/>
       <c r="K29" s="35"/>
@@ -4974,14 +5092,14 @@
         <v>72</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="F37" s="21" t="s">
         <v>134</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>135</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>5</v>
@@ -5207,10 +5325,10 @@
       </c>
       <c r="I45" s="13"/>
       <c r="J45" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K45" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5236,10 +5354,10 @@
       </c>
       <c r="I46" s="13"/>
       <c r="J46" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K46" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5265,10 +5383,10 @@
       </c>
       <c r="I47" s="13"/>
       <c r="J47" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K47" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5294,10 +5412,10 @@
       </c>
       <c r="I48" s="13"/>
       <c r="J48" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K48" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5323,10 +5441,10 @@
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K49" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5352,10 +5470,10 @@
       </c>
       <c r="I50" s="13"/>
       <c r="J50" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K50" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5381,10 +5499,10 @@
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K51" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5410,10 +5528,10 @@
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K52" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5439,10 +5557,10 @@
       </c>
       <c r="I53" s="13"/>
       <c r="J53" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K53" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5457,7 +5575,7 @@
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F54" s="30"/>
       <c r="G54" s="10" t="s">
@@ -5468,10 +5586,10 @@
       </c>
       <c r="I54" s="13"/>
       <c r="J54" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K54" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5486,7 +5604,7 @@
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F55" s="30"/>
       <c r="G55" s="10" t="s">
@@ -5497,10 +5615,10 @@
       </c>
       <c r="I55" s="13"/>
       <c r="J55" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K55" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5515,7 +5633,7 @@
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F56" s="30"/>
       <c r="G56" s="10" t="s">
@@ -5526,10 +5644,10 @@
       </c>
       <c r="I56" s="13"/>
       <c r="J56" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K56" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="9" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5543,7 +5661,7 @@
         <v>53</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F57" s="30"/>
       <c r="G57" s="10" t="s">
@@ -5554,10 +5672,10 @@
       </c>
       <c r="I57" s="13"/>
       <c r="J57" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K57" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5585,10 +5703,10 @@
       </c>
       <c r="I58" s="13"/>
       <c r="J58" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K58" s="36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -5599,14 +5717,23 @@
     <hyperlink ref="K26" r:id="rId3" xr:uid="{2A6DFCC8-01AB-4AEC-A71B-00449D86050B}"/>
     <hyperlink ref="K45" r:id="rId4" xr:uid="{D25DC240-F8DC-4212-B50A-5B4A03DF31D1}"/>
     <hyperlink ref="K46:K58" r:id="rId5" display="https://www.thingiverse.com/thing:4625509" xr:uid="{E0411AD5-806A-4606-A781-7174E5573058}"/>
+    <hyperlink ref="K5" r:id="rId6" xr:uid="{E6BDB980-958E-45BE-BEEE-5373B8D85381}"/>
+    <hyperlink ref="K6" r:id="rId7" xr:uid="{1928DF7C-C409-4053-BE71-9A54B4B841FA}"/>
+    <hyperlink ref="K4" r:id="rId8" xr:uid="{1B94BC14-F1C6-4D9D-9E46-4EC22C057135}"/>
+    <hyperlink ref="K10" r:id="rId9" xr:uid="{56CC717F-D564-4FB4-9DA0-89A1D458B38C}"/>
+    <hyperlink ref="K11" r:id="rId10" xr:uid="{AE9EB605-5EA9-450F-914A-4A275E5FD619}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{4A04A61F-89DF-4E5F-9086-F0637F5276FA}"/>
+    <hyperlink ref="K14" r:id="rId12" xr:uid="{F1BF7123-7265-4ED4-A5ED-BC89DA23DA99}"/>
+    <hyperlink ref="K18" r:id="rId13" xr:uid="{2910BA2F-EB1E-4CF0-BF0A-767DA0965AA0}"/>
+    <hyperlink ref="K20" r:id="rId14" xr:uid="{E7B9E93D-F8BA-4152-A490-A1CEC54B7B53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId15"/>
   <webPublishItems count="1">
     <webPublishItem id="10673" divId="BOM_XYHD12_10673" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_XYHD12.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HD BOM Qty of M6X14 Corrected.
</commit_message>
<xml_diff>
--- a/bom/BOM_XYHD12.xlsx
+++ b/bom/BOM_XYHD12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F52D8-30DC-468E-9866-7EE19291B0C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4BA5C5-7FEB-4CC7-A116-9A2D1C25B710}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="154">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -198,12 +198,6 @@
   </si>
   <si>
     <t>Shaft - 5X65mm</t>
-  </si>
-  <si>
-    <t>M5X12_ButtonHeadScrew_91239A228</t>
-  </si>
-  <si>
-    <t>Screw, ButtonHead - M5X12mm</t>
   </si>
   <si>
     <t>HevORT LOGO_Small_Grey</t>
@@ -349,9 +343,6 @@
     <t>Motor, Servo - Nema 23</t>
   </si>
   <si>
-    <t>https://www.teknic.com/model-info/CPM-SDSK-2321S-RQN/?model_voltage=75</t>
-  </si>
-  <si>
     <t>ClearPath by Teknic</t>
   </si>
   <si>
@@ -429,9 +420,6 @@
   <si>
     <t>*Length defined by Frame Calculator: https://miragec79.github.io/HevORT/framecalculator.html
 Look for HD X Cross Member into calculator</t>
-  </si>
-  <si>
-    <t>41</t>
   </si>
   <si>
     <t>M5X2020_T-Nut_91239A224</t>
@@ -515,12 +503,38 @@
   <si>
     <t>https://www.aliexpress.com/item/33002873710.html?spm=a2g0s.9042311.0.0.79334c4dbGMssZ</t>
   </si>
+  <si>
+    <t>EXPERIMENTAL</t>
+  </si>
+  <si>
+    <t>Stepper Motor - NEMA17X48mm</t>
+  </si>
+  <si>
+    <t>E3D
+LDO</t>
+  </si>
+  <si>
+    <t>High Output NEMA 17 0.9 degree can be used whith adapter plate:
+https://www.thingiverse.com/thing:4629296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option 1 </t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEMA17
+E3D_High_Torque_48mm or 
+LDO 60mm 0.9
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,6 +659,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -749,7 +779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -867,6 +897,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1119,13 +1161,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1207,13 +1249,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1251,13 +1293,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1427,13 +1469,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1691,13 +1733,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1867,13 +1909,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1911,13 +1953,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1955,13 +1997,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1999,13 +2041,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2043,13 +2085,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2087,13 +2129,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2131,13 +2173,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2175,13 +2217,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2263,13 +2305,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2351,13 +2393,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2439,13 +2481,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2527,13 +2569,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>927257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2571,50 +2613,6 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145117</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>154828</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>911412</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>927257</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 38" descr="thumbnail_38.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2274235" y="34116122"/>
-          <a:ext cx="766295" cy="772429"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>145117</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>154828</xdr:rowOff>
     </xdr:from>
@@ -2638,7 +2636,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2682,7 +2680,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2726,7 +2724,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2770,7 +2768,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2814,7 +2812,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2858,7 +2856,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2902,7 +2900,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2923,13 +2921,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>202268</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>224678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>965791</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>943869</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2946,7 +2944,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2967,13 +2965,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>202268</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>224678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>965791</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>943869</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2990,7 +2988,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3011,13 +3009,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>202268</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>224678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>965791</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>943869</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3034,7 +3032,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3055,13 +3053,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>202268</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>224678</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>965791</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>943869</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3078,7 +3076,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3122,7 +3120,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3166,7 +3164,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3210,7 +3208,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3254,7 +3252,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3298,7 +3296,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3342,7 +3340,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3386,7 +3384,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3407,13 +3405,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>122598</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>223798</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>971096</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>1054977</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3430,7 +3428,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3451,13 +3449,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>103844</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>224491</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>929550</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>1061300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3474,7 +3472,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3495,13 +3493,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>87967</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>116728</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1002866</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>985866</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3518,7 +3516,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3539,13 +3537,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>87967</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>116728</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1002866</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>985866</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3562,7 +3560,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3606,7 +3604,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3615,6 +3613,50 @@
         <a:xfrm>
           <a:off x="2098675" y="41760775"/>
           <a:ext cx="1031875" cy="983677"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1212850</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1143822</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 65" descr="thumbnail_24.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE4B2C93-588A-4744-B873-016457EC8ADE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2251075" y="14100175"/>
+          <a:ext cx="1069975" cy="1019997"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3972,8 +4014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="84.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3984,7 +4026,7 @@
     <col min="4" max="4" width="16.54296875" style="8" customWidth="1"/>
     <col min="5" max="5" width="44.7265625" style="16" customWidth="1"/>
     <col min="6" max="6" width="42.1796875" style="32" customWidth="1"/>
-    <col min="7" max="7" width="13" style="11" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" style="11" customWidth="1"/>
     <col min="8" max="8" width="9.1796875" style="11"/>
     <col min="9" max="9" width="60" style="29" customWidth="1"/>
     <col min="10" max="10" width="30" style="8" customWidth="1"/>
@@ -3994,13 +4036,13 @@
   <sheetData>
     <row r="1" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -4009,16 +4051,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -4029,7 +4071,7 @@
     </row>
     <row r="2" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>5</v>
@@ -4051,18 +4093,18 @@
         <v>2</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="9" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>5</v>
@@ -4072,10 +4114,10 @@
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>5</v>
@@ -4084,18 +4126,18 @@
         <v>1</v>
       </c>
       <c r="I3" s="31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="9" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>5</v>
@@ -4117,18 +4159,18 @@
         <v>4</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K4" s="38" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>5</v>
@@ -4138,10 +4180,10 @@
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G5" s="19" t="s">
         <v>5</v>
@@ -4150,18 +4192,18 @@
         <v>1</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J5" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K5" s="38" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>5</v>
@@ -4171,10 +4213,10 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>5</v>
@@ -4183,84 +4225,80 @@
         <v>1</v>
       </c>
       <c r="I6" s="31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K6" s="38" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>5</v>
+        <v>69</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>151</v>
       </c>
       <c r="C7" s="19">
         <v>6</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>5</v>
+        <v>102</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>147</v>
       </c>
       <c r="H7" s="12">
         <v>2</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="K7" s="36" t="s">
-        <v>105</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="K7" s="36"/>
     </row>
-    <row r="8" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="146" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>5</v>
+        <v>69</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="C8" s="19">
         <v>7</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="27">
-        <v>4</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="K8" s="33" t="s">
-        <v>136</v>
-      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="12">
+        <v>2</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J8" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="K8" s="40"/>
     </row>
     <row r="9" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>5</v>
@@ -4270,63 +4308,63 @@
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="26" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G9" s="24" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I9" s="37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="19">
         <v>9</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="12">
-        <v>4</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="J10" s="9" t="s">
+      <c r="D10" s="25"/>
+      <c r="E10" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="27">
+        <v>6</v>
+      </c>
+      <c r="I10" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="K10" s="36" t="s">
-        <v>140</v>
+      <c r="J10" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="K10" s="33" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>5</v>
@@ -4336,30 +4374,30 @@
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K11" s="36" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>5</v>
@@ -4369,28 +4407,30 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="30"/>
+        <v>75</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>73</v>
+      </c>
       <c r="G12" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K12" s="36" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>5</v>
@@ -4400,30 +4440,28 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>55</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F13" s="30"/>
       <c r="G13" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="K13" s="33" t="s">
-        <v>136</v>
+        <v>144</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>5</v>
@@ -4433,59 +4471,63 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="30" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="J14" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="K14" s="36" t="s">
-        <v>150</v>
+      <c r="J14" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="19">
         <v>14</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>80</v>
+      <c r="D15" s="9"/>
+      <c r="E15" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>86</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="34"/>
+      <c r="H15" s="12">
+        <v>2</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>5</v>
@@ -4495,26 +4537,26 @@
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="27" t="s">
-        <v>84</v>
-      </c>
       <c r="I16" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="34"/>
     </row>
     <row r="17" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>5</v>
@@ -4524,59 +4566,55 @@
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="27">
-        <v>3</v>
+      <c r="H17" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="I17" s="28" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J17" s="25"/>
       <c r="K17" s="34"/>
     </row>
     <row r="18" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="19">
         <v>17</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="12">
-        <v>4</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="K18" s="36" t="s">
-        <v>143</v>
-      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="27">
+        <v>3</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="34"/>
     </row>
     <row r="19" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>5</v>
@@ -4586,24 +4624,30 @@
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="30" t="s">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="F19" s="30" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="12">
-        <v>1</v>
-      </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="35"/>
+        <v>4</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="K19" s="36" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>5</v>
@@ -4613,254 +4657,254 @@
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="30" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="F20" s="30" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="12">
-        <v>2</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="K20" s="36" t="s">
-        <v>149</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I20" s="13"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="35"/>
     </row>
     <row r="21" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="19">
         <v>20</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="J21" s="25"/>
-      <c r="K21" s="34"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="12">
+        <v>2</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K21" s="36" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>5</v>
       </c>
       <c r="C22" s="19">
         <v>21</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="12">
-        <v>6</v>
-      </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="35"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="34"/>
     </row>
     <row r="23" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" s="19">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="30" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="12">
-        <v>24</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>123</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I23" s="13"/>
       <c r="J23" s="9"/>
       <c r="K23" s="35"/>
     </row>
     <row r="24" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C24" s="19">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="30" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="12">
-        <v>4</v>
-      </c>
-      <c r="I24" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>120</v>
+      </c>
       <c r="J24" s="9"/>
       <c r="K24" s="35"/>
     </row>
     <row r="25" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="19">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="30" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H25" s="12">
-        <v>8</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="K25" s="35" t="s">
-        <v>118</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="35"/>
     </row>
     <row r="26" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" s="19">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="30" t="s">
         <v>116</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H26" s="12">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C27" s="19">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="30" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H27" s="12">
-        <v>4</v>
-      </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="35"/>
+        <v>24</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="19">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H28" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="9"/>
@@ -4868,76 +4912,76 @@
     </row>
     <row r="29" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C29" s="19">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="30" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H29" s="12">
-        <v>8</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>121</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I29" s="13"/>
       <c r="J29" s="9"/>
       <c r="K29" s="35"/>
     </row>
     <row r="30" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C30" s="19">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="30" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="12">
-        <v>2</v>
-      </c>
-      <c r="I30" s="13"/>
+        <v>8</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>118</v>
+      </c>
       <c r="J30" s="9"/>
       <c r="K30" s="35"/>
     </row>
     <row r="31" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31" s="19">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="30" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>5</v>
@@ -4951,26 +4995,26 @@
     </row>
     <row r="32" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C32" s="19">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="30" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="12">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="I32" s="13"/>
       <c r="J32" s="9"/>
@@ -4978,26 +5022,26 @@
     </row>
     <row r="33" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="19">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="30" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="12">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="9"/>
@@ -5005,13 +5049,13 @@
     </row>
     <row r="34" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C34" s="19">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="30" t="s">
@@ -5032,13 +5076,13 @@
     </row>
     <row r="35" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" s="19">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="30" t="s">
@@ -5059,13 +5103,13 @@
     </row>
     <row r="36" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" s="19">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="30" t="s">
@@ -5086,20 +5130,20 @@
     </row>
     <row r="37" spans="1:11" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>132</v>
+        <v>70</v>
+      </c>
+      <c r="C37" s="19">
+        <v>36</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>5</v>
@@ -5113,13 +5157,13 @@
     </row>
     <row r="38" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="19">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="30" t="s">
@@ -5140,13 +5184,13 @@
     </row>
     <row r="39" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39" s="19">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="30" t="s">
@@ -5167,13 +5211,13 @@
     </row>
     <row r="40" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" s="19">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="30" t="s">
@@ -5194,13 +5238,13 @@
     </row>
     <row r="41" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="19">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="30" t="s">
@@ -5221,13 +5265,13 @@
     </row>
     <row r="42" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C42" s="19">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="30" t="s">
@@ -5248,13 +5292,13 @@
     </row>
     <row r="43" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C43" s="19">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="30" t="s">
@@ -5267,7 +5311,7 @@
         <v>5</v>
       </c>
       <c r="H43" s="12">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I43" s="13"/>
       <c r="J43" s="9"/>
@@ -5275,20 +5319,20 @@
     </row>
     <row r="44" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C44" s="19">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G44" s="10" t="s">
         <v>5</v>
@@ -5297,24 +5341,24 @@
         <v>4</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="35"/>
     </row>
     <row r="45" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C45" s="19">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F45" s="30"/>
       <c r="G45" s="10" t="s">
@@ -5325,25 +5369,25 @@
       </c>
       <c r="I45" s="13"/>
       <c r="J45" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K45" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="19">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F46" s="30"/>
       <c r="G46" s="10" t="s">
@@ -5354,21 +5398,21 @@
       </c>
       <c r="I46" s="13"/>
       <c r="J46" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K46" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="19">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="30" t="s">
@@ -5383,25 +5427,25 @@
       </c>
       <c r="I47" s="13"/>
       <c r="J47" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K47" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C48" s="19">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="10" t="s">
@@ -5412,21 +5456,21 @@
       </c>
       <c r="I48" s="13"/>
       <c r="J48" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K48" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C49" s="19">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="30" t="s">
@@ -5441,25 +5485,25 @@
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K49" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C50" s="19">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F50" s="30"/>
       <c r="G50" s="10" t="s">
@@ -5470,21 +5514,21 @@
       </c>
       <c r="I50" s="13"/>
       <c r="J50" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K50" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="19">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="30" t="s">
@@ -5499,25 +5543,25 @@
       </c>
       <c r="I51" s="13"/>
       <c r="J51" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K51" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B52" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C52" s="19">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="10" t="s">
@@ -5528,25 +5572,25 @@
       </c>
       <c r="I52" s="13"/>
       <c r="J52" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K52" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="19">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F53" s="30"/>
       <c r="G53" s="10" t="s">
@@ -5557,25 +5601,25 @@
       </c>
       <c r="I53" s="13"/>
       <c r="J53" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K53" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="19">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F54" s="30"/>
       <c r="G54" s="10" t="s">
@@ -5586,25 +5630,25 @@
       </c>
       <c r="I54" s="13"/>
       <c r="J54" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K54" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="19">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F55" s="30"/>
       <c r="G55" s="10" t="s">
@@ -5615,25 +5659,25 @@
       </c>
       <c r="I55" s="13"/>
       <c r="J55" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K55" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C56" s="19">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F56" s="30"/>
       <c r="G56" s="10" t="s">
@@ -5644,24 +5688,24 @@
       </c>
       <c r="I56" s="13"/>
       <c r="J56" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K56" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="9" customFormat="1" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="19">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F57" s="30"/>
       <c r="G57" s="10" t="s">
@@ -5672,28 +5716,28 @@
       </c>
       <c r="I57" s="13"/>
       <c r="J57" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K57" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="19">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F58" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G58" s="10" t="s">
         <v>13</v>
@@ -5703,31 +5747,31 @@
       </c>
       <c r="I58" s="13"/>
       <c r="J58" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K58" s="36" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K7" r:id="rId1" xr:uid="{B8E53FFD-F859-44E9-B35D-478F2ABD3E18}"/>
-    <hyperlink ref="K25" r:id="rId2" xr:uid="{4FC3AE5A-AD54-4717-A367-9016406F2CBF}"/>
-    <hyperlink ref="K26" r:id="rId3" xr:uid="{2A6DFCC8-01AB-4AEC-A71B-00449D86050B}"/>
-    <hyperlink ref="K45" r:id="rId4" xr:uid="{D25DC240-F8DC-4212-B50A-5B4A03DF31D1}"/>
-    <hyperlink ref="K46:K58" r:id="rId5" display="https://www.thingiverse.com/thing:4625509" xr:uid="{E0411AD5-806A-4606-A781-7174E5573058}"/>
-    <hyperlink ref="K5" r:id="rId6" xr:uid="{E6BDB980-958E-45BE-BEEE-5373B8D85381}"/>
-    <hyperlink ref="K6" r:id="rId7" xr:uid="{1928DF7C-C409-4053-BE71-9A54B4B841FA}"/>
-    <hyperlink ref="K4" r:id="rId8" xr:uid="{1B94BC14-F1C6-4D9D-9E46-4EC22C057135}"/>
-    <hyperlink ref="K10" r:id="rId9" xr:uid="{56CC717F-D564-4FB4-9DA0-89A1D458B38C}"/>
-    <hyperlink ref="K11" r:id="rId10" xr:uid="{AE9EB605-5EA9-450F-914A-4A275E5FD619}"/>
-    <hyperlink ref="K12" r:id="rId11" xr:uid="{4A04A61F-89DF-4E5F-9086-F0637F5276FA}"/>
-    <hyperlink ref="K14" r:id="rId12" xr:uid="{F1BF7123-7265-4ED4-A5ED-BC89DA23DA99}"/>
-    <hyperlink ref="K18" r:id="rId13" xr:uid="{2910BA2F-EB1E-4CF0-BF0A-767DA0965AA0}"/>
-    <hyperlink ref="K20" r:id="rId14" xr:uid="{E7B9E93D-F8BA-4152-A490-A1CEC54B7B53}"/>
+    <hyperlink ref="K26" r:id="rId1" xr:uid="{4FC3AE5A-AD54-4717-A367-9016406F2CBF}"/>
+    <hyperlink ref="K27" r:id="rId2" xr:uid="{2A6DFCC8-01AB-4AEC-A71B-00449D86050B}"/>
+    <hyperlink ref="K45" r:id="rId3" xr:uid="{D25DC240-F8DC-4212-B50A-5B4A03DF31D1}"/>
+    <hyperlink ref="K46:K58" r:id="rId4" display="https://www.thingiverse.com/thing:4625509" xr:uid="{E0411AD5-806A-4606-A781-7174E5573058}"/>
+    <hyperlink ref="K5" r:id="rId5" xr:uid="{E6BDB980-958E-45BE-BEEE-5373B8D85381}"/>
+    <hyperlink ref="K6" r:id="rId6" xr:uid="{1928DF7C-C409-4053-BE71-9A54B4B841FA}"/>
+    <hyperlink ref="K4" r:id="rId7" xr:uid="{1B94BC14-F1C6-4D9D-9E46-4EC22C057135}"/>
+    <hyperlink ref="K11" r:id="rId8" xr:uid="{56CC717F-D564-4FB4-9DA0-89A1D458B38C}"/>
+    <hyperlink ref="K12" r:id="rId9" xr:uid="{AE9EB605-5EA9-450F-914A-4A275E5FD619}"/>
+    <hyperlink ref="K13" r:id="rId10" xr:uid="{4A04A61F-89DF-4E5F-9086-F0637F5276FA}"/>
+    <hyperlink ref="K15" r:id="rId11" xr:uid="{F1BF7123-7265-4ED4-A5ED-BC89DA23DA99}"/>
+    <hyperlink ref="K19" r:id="rId12" xr:uid="{2910BA2F-EB1E-4CF0-BF0A-767DA0965AA0}"/>
+    <hyperlink ref="K21" r:id="rId13" xr:uid="{E7B9E93D-F8BA-4152-A490-A1CEC54B7B53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId14"/>
   <drawing r:id="rId15"/>
   <webPublishItems count="1">
     <webPublishItem id="10673" divId="BOM_XYHD12_10673" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_XYHD12.htm" autoRepublish="1"/>

</xml_diff>